<commit_message>
version 1.0 first usable version
</commit_message>
<xml_diff>
--- a/static/datafile/xmjd.xlsx
+++ b/static/datafile/xmjd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28035" windowHeight="10530" activeTab="14"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="28035" windowHeight="10530"/>
   </bookViews>
   <sheets>
     <sheet name="主要项目情况" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,15 @@
     <sheet name="云尚公司" sheetId="11" r:id="rId11"/>
     <sheet name="国际城" sheetId="13" r:id="rId12"/>
     <sheet name="兰草坝项目" sheetId="18" r:id="rId13"/>
-    <sheet name="贵阳市云岩国有投资控股集团" sheetId="19" r:id="rId14"/>
-    <sheet name="贵阳云岩贵中土地开发基本建设投资管理集团有限公司" sheetId="20" r:id="rId15"/>
+    <sheet name="贵中" sheetId="19" r:id="rId14"/>
+    <sheet name="贵阳云岩国有投资控股集团" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="192">
   <si>
     <t>序号</t>
   </si>
@@ -122,7 +122,7 @@
     <t>申报</t>
   </si>
   <si>
-    <t>评估报告已发送至分行卢仁鑫处，今日客调撰写进度，财务部分已完成，第一章节完成部分</t>
+    <t>该项目已在新一代新建储备项目，CP里面提评估，先需补充项目预评估表格，明日请领导签字后提至审核处</t>
   </si>
   <si>
     <t>贵州中交德余高速公路有限公司</t>
@@ -157,7 +157,7 @@
     <t>客户放款材料已初步整理，等待客户担保方签署担保协议。</t>
   </si>
   <si>
-    <t>贵州师范大学1</t>
+    <t>贵州师范大学</t>
   </si>
   <si>
     <t>固贷（新租贷）</t>
@@ -194,9 +194,6 @@
     <t>已累计投放1.68亿（其中我行1亿），剩余1.82亿预计年初投放（其中我行份额1.1亿）</t>
   </si>
   <si>
-    <t>贵州师范大学</t>
-  </si>
-  <si>
     <t>信用额度重检</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>撰写客调</t>
+  </si>
+  <si>
+    <t>评估报告已发送至分行卢仁鑫处，今日客调撰写进度，财务部分已完成，第一章节完成部分</t>
   </si>
   <si>
     <t>新签1.8亿贷款合同、集团担保合同</t>
@@ -539,6 +539,39 @@
   </si>
   <si>
     <t>已按要求写完评估报告，12.11与分行讨论，最后定稿</t>
+  </si>
+  <si>
+    <t>取得评估报告初稿</t>
+  </si>
+  <si>
+    <t>完成申报材料撰写</t>
+  </si>
+  <si>
+    <t>询问客户是否已获得项目初设批复</t>
+  </si>
+  <si>
+    <t>客户表示还未获得</t>
+  </si>
+  <si>
+    <t>持续跟踪客户行政要件获取情况，第一时间更新资料</t>
+  </si>
+  <si>
+    <t>额度申报书，单笔申报书，超风险限额申报书审核</t>
+  </si>
+  <si>
+    <t>已反馈修改意见，已完成超风险限额申报书修改</t>
+  </si>
+  <si>
+    <t>完成其他申报材料修改</t>
+  </si>
+  <si>
+    <t>与分行沟通评估报告初稿中资金缺口问题</t>
+  </si>
+  <si>
+    <t>已确认分行评估报告测算数据</t>
+  </si>
+  <si>
+    <t>就我行评估报告中资金缺口情况，与分行经营部门沟通解决办法</t>
   </si>
   <si>
     <t>申报阶段</t>
@@ -606,11 +639,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -678,16 +711,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -702,16 +742,61 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,39 +811,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,31 +825,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -821,7 +854,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,13 +986,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,73 +1010,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,67 +1028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,22 +1111,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1108,21 +1126,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1143,6 +1146,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1158,7 +1176,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1167,124 +1200,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1293,16 +1326,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1340,11 +1373,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1717,7 +1750,7 @@
   <sheetPr/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1835,7 +1868,7 @@
       </c>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" ht="27" spans="1:11">
+    <row r="4" ht="40.5" spans="1:11">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -2086,7 +2119,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>12</v>
@@ -2095,7 +2128,7 @@
         <v>18000</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>21</v>
@@ -2104,7 +2137,7 @@
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K12" s="16"/>
     </row>
@@ -2113,7 +2146,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>12</v>
@@ -2122,7 +2155,7 @@
         <v>5000</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>14</v>
@@ -2137,7 +2170,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" s="16"/>
     </row>
@@ -2146,7 +2179,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>12</v>
@@ -2168,7 +2201,7 @@
         <v>23</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" s="16"/>
     </row>
@@ -2177,7 +2210,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>12</v>
@@ -2186,10 +2219,10 @@
         <v>135000</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
@@ -2197,7 +2230,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="16"/>
     </row>
@@ -2206,7 +2239,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>12</v>
@@ -2215,7 +2248,7 @@
         <v>12000</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>37</v>
@@ -2228,7 +2261,7 @@
         <v>29</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K16" s="16"/>
     </row>
@@ -2237,7 +2270,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>12</v>
@@ -2246,7 +2279,7 @@
         <v>200000</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>37</v>
@@ -2261,7 +2294,7 @@
         <v>29</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K17" s="16"/>
     </row>
@@ -2270,7 +2303,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>12</v>
@@ -2279,10 +2312,10 @@
         <v>8000</v>
       </c>
       <c r="E18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>37</v>
@@ -2294,7 +2327,7 @@
         <v>29</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K18" s="16"/>
     </row>
@@ -2303,7 +2336,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>12</v>
@@ -2312,10 +2345,10 @@
         <v>10000</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>15</v>
@@ -2327,7 +2360,7 @@
         <v>23</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K19" s="16"/>
     </row>
@@ -2336,7 +2369,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -2345,7 +2378,7 @@
         <v>3000</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>32</v>
@@ -2357,7 +2390,7 @@
         <v>29</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2383,13 +2416,13 @@
   <sheetPr/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" topLeftCell="J2" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
+    <col min="1" max="1" width="9.125" style="2"/>
     <col min="2" max="2" width="14.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="34.5" style="2" customWidth="1"/>
@@ -2405,23 +2438,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2430,31 +2463,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2552,30 +2585,62 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="9">
+        <v>44179</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="A8" s="9">
+        <v>44180</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="4"/>
@@ -2793,23 +2858,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2818,31 +2883,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:11">
@@ -2850,22 +2915,22 @@
         <v>44166</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2911,23 +2976,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2936,31 +3001,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:11">
@@ -2968,24 +3033,24 @@
         <v>44175</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -3031,23 +3096,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="23.3" customHeight="1" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3056,31 +3121,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:11">
@@ -3088,26 +3153,26 @@
         <v>44175</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3140,23 +3205,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="23.3" customHeight="1" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3165,31 +3230,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3197,17 +3262,17 @@
         <v>44175</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3234,7 +3299,7 @@
   <sheetPr/>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3245,50 +3310,50 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>85</v>
-      </c>
-      <c r="I1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="23.3" customHeight="1" spans="1:11">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>88</v>
       </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
         <v>87</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="H2" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
         <v>87</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:11">
@@ -3296,15 +3361,15 @@
         <v>44175</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3335,7 +3400,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -3363,7 +3428,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="4:4">
@@ -3373,7 +3438,7 @@
     </row>
     <row r="5" spans="4:4">
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3410,23 +3475,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3435,56 +3500,56 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>44175</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -3770,23 +3835,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3795,31 +3860,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" ht="148.5" spans="1:11">
@@ -3829,32 +3894,32 @@
       <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" ht="67.5" spans="1:11">
@@ -3871,13 +3936,13 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -3887,20 +3952,20 @@
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -3917,11 +3982,11 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -4147,13 +4212,13 @@
   <sheetPr/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="D4" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
+    <col min="1" max="1" width="9.125" style="2"/>
     <col min="2" max="2" width="14.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
@@ -4169,23 +4234,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4194,31 +4259,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" ht="175.5" spans="1:11">
@@ -4229,25 +4294,25 @@
         <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" ht="27" spans="1:11">
@@ -4257,8 +4322,8 @@
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>119</v>
+      <c r="C4" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -4283,13 +4348,13 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" ht="135" spans="1:11">
@@ -4303,22 +4368,28 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="9" t="s">
-        <v>30</v>
+      <c r="G6" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+    <row r="7" ht="162" spans="1:11">
+      <c r="A7" s="9">
+        <v>44180</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -4553,23 +4624,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4578,31 +4649,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4622,12 +4693,12 @@
         <v>125</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -4913,23 +4984,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4938,31 +5009,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4973,12 +5044,12 @@
         <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -5271,23 +5342,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5296,31 +5367,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5624,23 +5695,23 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="17.25" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5649,31 +5720,31 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="I2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" ht="67.5" spans="1:11">
@@ -5681,28 +5752,28 @@
         <v>44172</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>138</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -5720,10 +5791,10 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="10" t="s">
         <v>141</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -5741,13 +5812,13 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>145</v>
       </c>
     </row>
@@ -5762,10 +5833,10 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>147</v>
       </c>
       <c r="K6" s="4"/>

</xml_diff>